<commit_message>
Updated code on 3-8-21
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestConfiguration.xlsx
+++ b/src/test/resources/TestData/TestConfiguration.xlsx
@@ -120,9 +120,6 @@
     <t>ReportPath</t>
   </si>
   <si>
-    <t>X:/AMPS Data/MobileAutomationReports/</t>
-  </si>
-  <si>
     <t>Excel</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>RealDevice</t>
+  </si>
+  <si>
+    <t>C:/Users/yogesha/Desktop/TreatApp WorkSpace/Mobile/MobileAutomationTestReports/</t>
   </si>
 </sst>
 </file>
@@ -221,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -244,12 +244,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -298,6 +365,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -637,15 +721,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="40" style="3" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="85.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -711,7 +795,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3"/>
     </row>
@@ -721,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4"/>
     </row>
@@ -749,7 +833,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7"/>
     </row>
@@ -769,25 +853,25 @@
     </row>
     <row r="10" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="26" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="25" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -800,16 +884,16 @@
         <v>26</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -869,17 +953,17 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="13"/>
+      <c r="C21" s="21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>33</v>
+      <c r="C22" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
@@ -893,8 +977,8 @@
       <c r="B23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>38</v>
+      <c r="C23" s="22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -905,7 +989,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
IOs and Android Update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestConfiguration.xlsx
+++ b/src/test/resources/TestData/TestConfiguration.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="6135" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -84,9 +84,6 @@
     <t>newCommandTimeout</t>
   </si>
   <si>
-    <t>iOS</t>
-  </si>
-  <si>
     <t>Sauce Details</t>
   </si>
   <si>
@@ -129,10 +126,6 @@
     <t>Thrivent-debug.ipa</t>
   </si>
   <si>
-    <t xml:space="preserve">iPhone 12
-</t>
-  </si>
-  <si>
     <t>./src/test/resources/TestData/TestCaseSettings.xlsx</t>
   </si>
   <si>
@@ -145,10 +138,19 @@
     <t>app-qa-release.apk</t>
   </si>
   <si>
+    <t>C:/Users/yogesha/Desktop/TreatApp WorkSpace/Mobile/MobileAutomationTestReports/</t>
+  </si>
+  <si>
+    <t>./MobileAutomationTestReports/</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
     <t>RealDevice</t>
   </si>
   <si>
-    <t>C:/Users/yogesha/Desktop/TreatApp WorkSpace/Mobile/MobileAutomationTestReports/</t>
+    <t>Android</t>
   </si>
 </sst>
 </file>
@@ -356,9 +358,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -382,6 +381,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -719,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN30"/>
+  <dimension ref="A1:AM30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +732,10 @@
     <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="40" style="3" customWidth="1"/>
     <col min="3" max="3" width="85.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9" style="3"/>
+    <col min="4" max="6" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -745,7 +747,7 @@
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="F1"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -779,129 +781,129 @@
       <c r="AK1"/>
       <c r="AL1"/>
       <c r="AM1"/>
-      <c r="AN1"/>
-    </row>
-    <row r="2" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="11"/>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:40" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="12"/>
-      <c r="G6"/>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7"/>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="13"/>
-      <c r="G8"/>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="13"/>
-      <c r="G9"/>
-    </row>
-    <row r="10" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="28" t="s">
+      <c r="B10" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C10" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="12"/>
     </row>
-    <row r="16" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>8</v>
       </c>
@@ -911,9 +913,8 @@
       <c r="C16" s="13">
         <v>90</v>
       </c>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="9" t="s">
         <v>19</v>
@@ -922,7 +923,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="9" t="s">
         <v>9</v>
@@ -930,9 +931,8 @@
       <c r="C18" s="13">
         <v>10</v>
       </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="9" t="s">
         <v>10</v>
@@ -941,7 +941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="9" t="s">
         <v>11</v>
@@ -949,39 +949,41 @@
       <c r="C20" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L20" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>42</v>
+      <c r="C22" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>6</v>
       </c>
@@ -989,43 +991,43 @@
         <v>7</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="13"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="9" t="s">
         <v>18</v>
@@ -1034,12 +1036,15 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>"Excel,Database"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>"Cloud,RealDevice"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>"iOS,Android"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51" footer="0.51"/>

</xml_diff>